<commit_message>
Adicionado loop para pular células no excel e variáveis para controlar quantas linhas queremos
</commit_message>
<xml_diff>
--- a/Teste.xlsx
+++ b/Teste.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Desktop\Organizar\APS 4°Semestre\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Desktop\Organizar\APS-4-Semestre\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Nome</t>
   </si>
@@ -33,6 +33,24 @@
   </si>
   <si>
     <t>Will</t>
+  </si>
+  <si>
+    <t>País</t>
+  </si>
+  <si>
+    <t>Brasil</t>
+  </si>
+  <si>
+    <t>ChingChongBingBong</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Kyle</t>
+  </si>
+  <si>
+    <t>US</t>
   </si>
 </sst>
 </file>
@@ -350,28 +368,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>